<commit_message>
14 October assignment commited
</commit_message>
<xml_diff>
--- a/AssignmentProject/MobileData/testData.xlsx
+++ b/AssignmentProject/MobileData/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>All active projects of all active customers</t>
   </si>
@@ -204,9 +204,6 @@
     <t>itemName</t>
   </si>
   <si>
-    <t>fav7</t>
-  </si>
-  <si>
     <t>123456</t>
   </si>
   <si>
@@ -235,6 +232,21 @@
   </si>
   <si>
     <t>M.A.C Satin Lipstick - Mocha</t>
+  </si>
+  <si>
+    <t>Fav10</t>
+  </si>
+  <si>
+    <t>M.A.C Matte Lipstick - Mehr</t>
+  </si>
+  <si>
+    <t>expectedMsg</t>
+  </si>
+  <si>
+    <t>Your Shopping Bag is Empty</t>
+  </si>
+  <si>
+    <t>M.A.C Cremesheen Lipstick - Creme In Your Coffee</t>
   </si>
 </sst>
 </file>
@@ -864,7 +876,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -872,7 +884,7 @@
     <col min="1" max="1" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -933,7 +945,7 @@
         <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>49</v>
@@ -952,7 +964,7 @@
         <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -966,53 +978,74 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
         <v>70</v>
       </c>
-      <c r="E2" t="s">
-        <v>71</v>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="E6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Task for 15-Oct-2020 Completed
</commit_message>
<xml_diff>
--- a/AssignmentProject/MobileData/testData.xlsx
+++ b/AssignmentProject/MobileData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6435" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6435" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="EcommData" sheetId="5" r:id="rId5"/>
     <sheet name="NykaaData" sheetId="6" r:id="rId6"/>
+    <sheet name="AccountCreation" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="104">
   <si>
     <t>All active projects of all active customers</t>
   </si>
@@ -247,6 +248,90 @@
   </si>
   <si>
     <t>M.A.C Cremesheen Lipstick - Creme In Your Coffee</t>
+  </si>
+  <si>
+    <t>For Validation of Shade</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>Nykaa Naturals</t>
+  </si>
+  <si>
+    <t>Nykaa Skin Potion Facial Oil</t>
+  </si>
+  <si>
+    <t>Rs. 500 - Rs. 999</t>
+  </si>
+  <si>
+    <t>Nykaa Naturals Facial Oil - Pure Cold Pressed</t>
+  </si>
+  <si>
+    <t>Preference Filter</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Concern filter</t>
+  </si>
+  <si>
+    <t>Dullness</t>
+  </si>
+  <si>
+    <t>ShadeName</t>
+  </si>
+  <si>
+    <t>Argan</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>462001</t>
+  </si>
+  <si>
+    <t>Philips Beard Trimmer BT3101/15</t>
+  </si>
+  <si>
+    <t>email id</t>
+  </si>
+  <si>
+    <t>Pagination page</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>expectedSuccessNotificationMsg</t>
+  </si>
+  <si>
+    <t>You are subscribed to this notification.</t>
+  </si>
+  <si>
+    <t>8109388546</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>departmentName</t>
+  </si>
+  <si>
+    <t>sajal</t>
+  </si>
+  <si>
+    <t>jain</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
@@ -299,11 +384,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -978,74 +1064,219 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="E3" t="s">
+    <row r="3" spans="1:7">
+      <c r="E3" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="E6" t="s">
+    <row r="6" spans="1:7">
+      <c r="E6" s="1" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>